<commit_message>
last update data class 6
</commit_message>
<xml_diff>
--- a/reporte_estabilidad_psi_comite.xlsx
+++ b/reporte_estabilidad_psi_comite.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,41 +451,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.004327109561719563</v>
+        <v>8.708494321115293</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00361919785439588</v>
+        <v>8.499745816355652</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003076724471026956</v>
+        <v>0.004354313091303515</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -496,11 +496,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.003042683317760516</v>
+        <v>0.00361919785439588</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -511,11 +511,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001837675422419448</v>
+        <v>0.003076724471026956</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -526,11 +526,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001331679411860989</v>
+        <v>0.003042683317760516</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -541,11 +541,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.001306469329722873</v>
+        <v>0.002485986357051597</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -556,11 +556,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.001001141559916685</v>
+        <v>0.001837675422419448</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -571,11 +571,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0001556094088038086</v>
+        <v>0.001359399605215724</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -586,11 +586,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0001142621172110512</v>
+        <v>0.001294207085647241</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -601,11 +601,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.844856427447264e-05</v>
+        <v>0.001121697744503871</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -616,13 +616,43 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>num_lineas</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0001142621172110512</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>max_mora_12m</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2.844856427447264e-05</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>mora_30d_12m</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B15" t="n">
         <v>0</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -639,7 +669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,10 +721,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4953438128585264</v>
+        <v>0.4901946328516662</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4964365256124721</v>
+        <v>0.4925966850828729</v>
       </c>
       <c r="D2" t="n">
         <v>0.181455858023763</v>
@@ -703,7 +733,7 @@
         <v>0.1799013010318528</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001092712753945735</v>
+        <v>0.002402052231206708</v>
       </c>
       <c r="G2" t="n">
         <v>-0.001554556991910122</v>
@@ -716,10 +746,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2984057215227595</v>
+        <v>0.2953037452079033</v>
       </c>
       <c r="C3" t="n">
-        <v>0.289532293986637</v>
+        <v>0.287292817679558</v>
       </c>
       <c r="D3" t="n">
         <v>0.1750093621270753</v>
@@ -728,7 +758,7 @@
         <v>0.1823076923076923</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.008873427536122469</v>
+        <v>-0.008010927528345257</v>
       </c>
       <c r="G3" t="n">
         <v>0.007298330180617041</v>
@@ -741,10 +771,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1490724875214185</v>
+        <v>0.1475228546151578</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1481069042316258</v>
+        <v>0.1469613259668508</v>
       </c>
       <c r="D4" t="n">
         <v>0.1766616691654173</v>
@@ -753,7 +783,7 @@
         <v>0.1819548872180451</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0009655832897926264</v>
+        <v>-0.0005615286483069415</v>
       </c>
       <c r="G4" t="n">
         <v>0.005293218052627835</v>
@@ -766,10 +796,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04775385532295314</v>
+        <v>0.04725744618106753</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05478841870824053</v>
+        <v>0.0543646408839779</v>
       </c>
       <c r="D5" t="n">
         <v>0.1778471138845554</v>
@@ -778,7 +808,7 @@
         <v>0.1422764227642276</v>
       </c>
       <c r="F5" t="n">
-        <v>0.007034563385287393</v>
+        <v>0.007107194702910373</v>
       </c>
       <c r="G5" t="n">
         <v>-0.03557069112032774</v>
@@ -787,100 +817,125 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Digital </t>
+          <t>__MISSING__</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.00525217909558221</v>
+        <v>0.01039516366853436</v>
       </c>
       <c r="C6" t="n">
-        <v>0.005790645879732739</v>
+        <v>0.007734806629834255</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1560283687943262</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2692307692307692</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0005384667841505297</v>
+        <v>-0.002660357038700101</v>
       </c>
       <c r="G6" t="n">
-        <v>0.113202400436443</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tienda </t>
+          <t xml:space="preserve"> Digital </t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.002272219325039112</v>
+        <v>0.005197581834267178</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00311804008908686</v>
+        <v>0.00574585635359116</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1147540983606557</v>
+        <v>0.1560283687943262</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.2692307692307692</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0008458207640477475</v>
+        <v>0.0005482745193239828</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02810304449648711</v>
+        <v>0.113202400436443</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FuerzaVenta </t>
+          <t xml:space="preserve"> Tienda </t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.001340981896744394</v>
+        <v>0.002248599233264524</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00178173719376392</v>
+        <v>0.003093922651933702</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.1147540983606557</v>
       </c>
       <c r="E8" t="n">
-        <v>0.375</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0004407552970195259</v>
+        <v>0.0008453234186691781</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1527777777777778</v>
+        <v>0.02810304449648711</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t xml:space="preserve"> FuerzaVenta </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.001327042170451194</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.001767955801104972</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0004409136306537781</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1527777777777778</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Alianza </t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0.0005587424569768308</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.00044543429844098</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B10" t="n">
+        <v>0.0005529342376879977</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0004419889502762431</v>
+      </c>
+      <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="n">
-        <v>-0.0001133081585358508</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="F10" t="n">
+        <v>-0.0001109452874117546</v>
+      </c>
+      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -895,7 +950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,10 +1002,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5519040166927491</v>
+        <v>0.5460041285756414</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5409141583054626</v>
+        <v>0.5361325966850828</v>
       </c>
       <c r="D2" t="n">
         <v>0.1780988387793681</v>
@@ -959,7 +1014,7 @@
         <v>0.1739488870568838</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0109898583872865</v>
+        <v>-0.00987153189055856</v>
       </c>
       <c r="G2" t="n">
         <v>-0.004149951722484307</v>
@@ -972,10 +1027,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4480959833072509</v>
+        <v>0.443305809495724</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4590858416945374</v>
+        <v>0.4550276243093923</v>
       </c>
       <c r="D3" t="n">
         <v>0.1768667886246466</v>
@@ -984,10 +1039,35 @@
         <v>0.1894123360854784</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01098985838728644</v>
+        <v>0.0117218148136683</v>
       </c>
       <c r="G3" t="n">
         <v>0.01254554746083178</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>__MISSING__</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01069006192863462</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.008839779005524863</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.001850282923109759</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1081,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,41 +1109,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.003987154065962509</v>
+        <v>8.701105049195897</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003620504236813012</v>
+        <v>8.430020953441606</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003190844102216097</v>
+        <v>0.003987154065962509</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1074,11 +1154,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.003147514010150547</v>
+        <v>0.003598433521704606</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1089,11 +1169,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.002987884821966549</v>
+        <v>0.003190844102216097</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1104,11 +1184,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.002777107147041426</v>
+        <v>0.003147514010150547</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1119,11 +1199,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.001714378914625647</v>
+        <v>0.002987884821966549</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1134,11 +1214,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0008497071122585257</v>
+        <v>0.002929642020525461</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1149,11 +1229,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004873266748798742</v>
+        <v>0.002492463086893575</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1164,11 +1244,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.000312455294370932</v>
+        <v>0.0008446377455223037</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1179,11 +1259,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6.39202814495119e-05</v>
+        <v>0.0008376767426752846</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1194,13 +1274,43 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>num_lineas</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.000312455294370932</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>max_mora_12m</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>6.39202814495119e-05</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>mora_30d_12m</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B15" t="n">
         <v>0</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1217,7 +1327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1250,15 +1360,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02760655644139679</v>
+        <v>9.813729380479312</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1268,15 +1378,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.009822678140185228</v>
+        <v>9.653086573752763</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1286,11 +1396,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.007586858227964241</v>
+        <v>0.02817817895709276</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1304,11 +1414,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.006810228922886923</v>
+        <v>0.009822678140185228</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1322,11 +1432,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.005522757622243576</v>
+        <v>0.007846564229482563</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1340,11 +1450,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.005476617239310443</v>
+        <v>0.007586858227964241</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1358,11 +1468,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.003402555877303438</v>
+        <v>0.006119015564907035</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1376,11 +1486,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.002420935412809033</v>
+        <v>0.005522757622243576</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1394,11 +1504,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.001209951815616341</v>
+        <v>0.005476617239310443</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1412,11 +1522,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>num_lineas</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001051536747610013</v>
+        <v>0.003402555877303438</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1430,11 +1540,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0002115928565579809</v>
+        <v>0.00271783773600119</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1448,11 +1558,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>mora_30d_12m</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.001529331727138495</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1466,11 +1576,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>max_mora_12m</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01041363225881701</v>
+        <v>0.0002115928565579809</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1478,17 +1588,17 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>202505</v>
+        <v>202504</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>mora_30d_12m</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.009821205920731785</v>
+        <v>0</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1496,21 +1606,21 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>202505</v>
+        <v>202504</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.007292555424739831</v>
+        <v>9.809207517888929</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1520,15 +1630,15 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.007070080281724043</v>
+        <v>9.630695706675986</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1538,11 +1648,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.005091220971740665</v>
+        <v>0.01041363225881701</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1556,11 +1666,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.003883073851303597</v>
+        <v>0.009821205920731785</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1574,11 +1684,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003512371345153793</v>
+        <v>0.007230538112754581</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1592,11 +1702,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.002467990441770625</v>
+        <v>0.007070080281724043</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1610,11 +1720,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.001973475364586123</v>
+        <v>0.005048869276873264</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1628,11 +1738,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.0003359576660003701</v>
+        <v>0.004449367466746451</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1646,11 +1756,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.0002675409970670659</v>
+        <v>0.003906504079667279</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1664,11 +1774,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>mora_30d_12m</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.003883073851303597</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1682,11 +1792,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>num_lineas</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.01163924759140547</v>
+        <v>0.002467990441770625</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1694,17 +1804,17 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>202506</v>
+        <v>202505</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.008336408102370825</v>
+        <v>0.0003895617028132475</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1712,17 +1822,17 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>202506</v>
+        <v>202505</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>max_mora_12m</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.007371669574021537</v>
+        <v>0.0002675409970670659</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1730,17 +1840,17 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>202506</v>
+        <v>202505</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>mora_30d_12m</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.006822059734882943</v>
+        <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1748,21 +1858,21 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>202506</v>
+        <v>202505</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.005847607329190953</v>
+        <v>9.77894811426194</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1772,15 +1882,15 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.004964327864654911</v>
+        <v>9.588838453774169</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1790,11 +1900,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.002203081783801443</v>
+        <v>0.01163924759140547</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1808,11 +1918,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.002157300475927798</v>
+        <v>0.008336408102370825</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1826,11 +1936,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.001650802383807138</v>
+        <v>0.007371669574021537</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1844,11 +1954,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.0008496295669922671</v>
+        <v>0.006752708830642405</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1862,11 +1972,11 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.0005454052569983156</v>
+        <v>0.005847607329190953</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1880,11 +1990,11 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>mora_30d_12m</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>0.005162792078019696</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1898,11 +2008,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.01100572053669482</v>
+        <v>0.002824824660937445</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1910,17 +2020,17 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>202507</v>
+        <v>202506</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>max_mora_12m</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.009579258217565959</v>
+        <v>0.002157300475927798</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1928,17 +2038,17 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>202507</v>
+        <v>202506</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.008997072487527</v>
+        <v>0.001954029201459337</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1946,17 +2056,17 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>202507</v>
+        <v>202506</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>num_lineas</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.005831124314020318</v>
+        <v>0.001650802383807138</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1964,17 +2074,17 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>202507</v>
+        <v>202506</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.003698361671851656</v>
+        <v>0.0009923171358854795</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1982,17 +2092,17 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>202507</v>
+        <v>202506</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>mora_30d_12m</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.003098540458746835</v>
+        <v>0</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2000,21 +2110,21 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>202507</v>
+        <v>202506</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.002329316535541961</v>
+        <v>9.769302391620773</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -2024,15 +2134,15 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.002272408396718432</v>
+        <v>9.527682559622928</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2042,11 +2152,11 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.002234718560847915</v>
+        <v>0.01100572053669482</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2060,11 +2170,11 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.0001382258500254533</v>
+        <v>0.009579258217565959</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2078,11 +2188,11 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4.417039304517838e-06</v>
+        <v>0.009178903129621616</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2096,11 +2206,11 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>mora_30d_12m</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>0.007300979571351516</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2114,11 +2224,11 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.01764451014821301</v>
+        <v>0.005831124314020318</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2126,7 +2236,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="51">
@@ -2136,7 +2246,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.008857592263643226</v>
+        <v>0.004672217282000289</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2144,17 +2254,17 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>num_lineas</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.007030018698600583</v>
+        <v>0.003698361671851656</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2162,17 +2272,17 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.006859321676325462</v>
+        <v>0.003098540458746835</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2180,17 +2290,17 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.00595251427848241</v>
+        <v>0.002312404974132645</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2198,17 +2308,17 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.005676135318352436</v>
+        <v>0.0008049608178772695</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2216,17 +2326,17 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>max_mora_12m</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.00558636324150538</v>
+        <v>0.0001382258500254533</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2234,17 +2344,17 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>mora_30d_12m</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.003734971506329647</v>
+        <v>0</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -2252,21 +2362,21 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>202508</v>
+        <v>202507</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.00357655974620647</v>
+        <v>9.793557377149684</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -2276,15 +2386,15 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.0008326526929691762</v>
+        <v>9.550057110450377</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -2294,11 +2404,11 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0003076915303947961</v>
+        <v>0.01764451014821301</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2312,11 +2422,11 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>mora_30d_12m</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>0.01049386702513088</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2330,11 +2440,11 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.009967252764366769</v>
+        <v>0.007434364637026594</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2342,17 +2452,17 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.006694077059828168</v>
+        <v>0.007030018698600583</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2360,17 +2470,17 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.004586267622141163</v>
+        <v>0.00613710648037142</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2378,17 +2488,17 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.004567481912071003</v>
+        <v>0.005767745210830827</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2396,17 +2506,17 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.003946427336587101</v>
+        <v>0.005676135318352436</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2414,17 +2524,17 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.003435561325649315</v>
+        <v>0.003734971506329647</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2432,17 +2542,17 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.002700814710485193</v>
+        <v>0.003566310086692267</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2450,17 +2560,17 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>num_lineas</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.002643163583544959</v>
+        <v>0.0008326526929691762</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2468,17 +2578,17 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>max_mora_12m</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.002189745877146796</v>
+        <v>0.0003076915303947961</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2486,17 +2596,17 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>mora_30d_12m</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.000324346304152139</v>
+        <v>0</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2504,21 +2614,21 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>202509</v>
+        <v>202508</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>7.145596661792925e-05</v>
+        <v>9.808856675158371</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2528,18 +2638,234 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>ingreso_mensual</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>9.553425324322331</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ALERT</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>score_bureau</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.009967252764366769</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>antig_banca_anios</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.006694077059828168</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>edad</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.004586267622141163</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>canal_origen</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.004523420838850861</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>segmento</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.003915650796004598</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>producto_principal</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.003619145667143954</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.002852335107743226</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>antig_laboral_anios</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.002700814710485193</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>num_lineas</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.002189745877146796</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>sexo</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.001388543537112751</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>max_mora_12m</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.000324346304152139</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>202509</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>mora_30d_12m</t>
         </is>
       </c>
-      <c r="B73" t="n">
+      <c r="B85" t="n">
         <v>0</v>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="D73" t="n">
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
         <v>202509</v>
       </c>
     </row>
@@ -2854,7 +3180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2873,6 +3199,11 @@
           <t>psi_target</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2881,6 +3212,11 @@
       <c r="B2" t="n">
         <v>0.004138105211389654</v>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -2889,6 +3225,11 @@
       <c r="B3" t="n">
         <v>9.977996614856903e-05</v>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -2897,6 +3238,11 @@
       <c r="B4" t="n">
         <v>0.0003980576468867939</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -2905,6 +3251,11 @@
       <c r="B5" t="n">
         <v>0.001234076993404024</v>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -2913,6 +3264,11 @@
       <c r="B6" t="n">
         <v>0.0002887337930640765</v>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -2920,6 +3276,11 @@
       </c>
       <c r="B7" t="n">
         <v>5.558367778779294e-07</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2933,7 +3294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2966,15 +3327,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.003987154065962509</v>
+        <v>8.701105049195897</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2986,15 +3347,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003620504236813012</v>
+        <v>8.430020953441606</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3006,11 +3367,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MIX::region</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003620504236813012</v>
+        <v>0.003987154065962509</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -3026,11 +3387,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.003190844102216097</v>
+        <v>0.003598433521704606</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -3046,11 +3407,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>MIX::region</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.003147514010150547</v>
+        <v>0.003598433521704606</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -3066,11 +3427,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.002987884821966549</v>
+        <v>0.003190844102216097</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -3086,11 +3447,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.002777107147041426</v>
+        <v>0.003147514010150547</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -3106,11 +3467,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MIX::segmento</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.002777107147041426</v>
+        <v>0.002987884821966549</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -3126,11 +3487,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.001714378914625647</v>
+        <v>0.002929642020525461</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -3146,11 +3507,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MIX::canal_origen</t>
+          <t>MIX::segmento</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001714378914625647</v>
+        <v>0.002929642020525461</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -3166,11 +3527,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0008497071122585257</v>
+        <v>0.002492463086893575</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -3186,11 +3547,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MIX::producto_principal</t>
+          <t>MIX::canal_origen</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0008497071122585257</v>
+        <v>0.002492463086893575</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -3206,11 +3567,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0004873266748798742</v>
+        <v>0.0008446377455223037</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -3226,11 +3587,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MIX::sexo</t>
+          <t>MIX::producto_principal</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0004873266748798742</v>
+        <v>0.0008446377455223037</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -3246,11 +3607,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.000312455294370932</v>
+        <v>0.0008376767426752846</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -3266,11 +3627,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>MIX::sexo</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6.39202814495119e-05</v>
+        <v>0.0008376767426752846</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -3286,11 +3647,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>mora_30d_next3m</t>
+          <t>num_lineas</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.153033327974173e-05</v>
+        <v>0.000312455294370932</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -3306,11 +3667,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>mora_30d_12m</t>
+          <t>max_mora_12m</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>6.39202814495119e-05</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -3326,11 +3687,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>mora_30d_next3m</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.004327109561719563</v>
+        <v>4.153033327974173e-05</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -3339,18 +3700,18 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>TRAIN_vs_TEST</t>
+          <t>TRAIN_vs_OOT</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MIX::region</t>
+          <t>mora_30d_12m</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.004327109561719563</v>
+        <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -3359,22 +3720,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TRAIN_vs_TEST</t>
+          <t>TRAIN_vs_OOT</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>score_bureau</t>
+          <t>utilizacion_tc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.00361919785439588</v>
+        <v>8.708494321115293</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -3386,15 +3747,15 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>antig_laboral_anios</t>
+          <t>ingreso_mensual</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.003076724471026956</v>
+        <v>8.499745816355652</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>ALERT</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -3406,11 +3767,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>region</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.003042683317760516</v>
+        <v>0.004354313091303515</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -3426,11 +3787,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>antig_banca_anios</t>
+          <t>MIX::region</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.001837675422419448</v>
+        <v>0.004354313091303515</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -3446,11 +3807,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>producto_principal</t>
+          <t>score_bureau</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.001331679411860989</v>
+        <v>0.00361919785439588</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -3466,11 +3827,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MIX::producto_principal</t>
+          <t>antig_laboral_anios</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.001331679411860989</v>
+        <v>0.003076724471026956</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -3486,11 +3847,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>segmento</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.001306469329722873</v>
+        <v>0.003042683317760516</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -3506,11 +3867,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MIX::segmento</t>
+          <t>canal_origen</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.001306469329722873</v>
+        <v>0.002485986357051597</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -3526,11 +3887,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>canal_origen</t>
+          <t>MIX::canal_origen</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.001001141559916685</v>
+        <v>0.002485986357051597</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -3546,11 +3907,11 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MIX::canal_origen</t>
+          <t>antig_banca_anios</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.001001141559916685</v>
+        <v>0.001837675422419448</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -3566,11 +3927,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>mora_30d_next3m</t>
+          <t>producto_principal</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.000308416335956975</v>
+        <v>0.001359399605215724</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -3586,11 +3947,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>MIX::producto_principal</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.0001556094088038086</v>
+        <v>0.001359399605215724</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -3606,11 +3967,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MIX::sexo</t>
+          <t>segmento</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0001556094088038086</v>
+        <v>0.001294207085647241</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -3626,11 +3987,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>num_lineas</t>
+          <t>MIX::segmento</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.0001142621172110512</v>
+        <v>0.001294207085647241</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -3646,11 +4007,11 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>max_mora_12m</t>
+          <t>sexo</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.844856427447264e-05</v>
+        <v>0.001121697744503871</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -3666,18 +4027,98 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>MIX::sexo</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.001121697744503871</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>TRAIN_vs_TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>mora_30d_next3m</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.000308416335956975</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>TRAIN_vs_TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>num_lineas</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.0001142621172110512</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>TRAIN_vs_TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>max_mora_12m</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2.844856427447264e-05</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>TRAIN_vs_TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>mora_30d_12m</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B41" t="n">
         <v>0</v>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
         <is>
           <t>TRAIN_vs_TEST</t>
         </is>
@@ -3694,7 +4135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3746,10 +4187,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4430780696851127</v>
+        <v>0.4382925390740194</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4287628405538187</v>
+        <v>0.4243093922651934</v>
       </c>
       <c r="D2" t="n">
         <v>0.1816652649285113</v>
@@ -3758,7 +4199,7 @@
         <v>0.1729166666666667</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.01431522913129402</v>
+        <v>-0.01398314680882606</v>
       </c>
       <c r="G2" t="n">
         <v>-0.008748598261844681</v>
@@ -3771,10 +4212,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1802869386994597</v>
+        <v>0.1783397227956355</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1822242072353729</v>
+        <v>0.1803314917127072</v>
       </c>
       <c r="D3" t="n">
         <v>0.1688714344770566</v>
@@ -3783,7 +4224,7 @@
         <v>0.1764705882352941</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001937268535913278</v>
+        <v>0.001991768917071673</v>
       </c>
       <c r="G3" t="n">
         <v>0.007599153758237498</v>
@@ -3796,10 +4237,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1666480342835849</v>
+        <v>0.1648481273960484</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1779812416257258</v>
+        <v>0.1761325966850829</v>
       </c>
       <c r="D4" t="n">
         <v>0.1791144901610018</v>
@@ -3808,7 +4249,7 @@
         <v>0.1819322459222083</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01133320734214088</v>
+        <v>0.01128446928903451</v>
       </c>
       <c r="G4" t="n">
         <v>0.002817755761206492</v>
@@ -3821,10 +4262,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1395192845164897</v>
+        <v>0.1380123857269242</v>
       </c>
       <c r="C5" t="n">
-        <v>0.141134435015632</v>
+        <v>0.1396685082872928</v>
       </c>
       <c r="D5" t="n">
         <v>0.1776175213675214</v>
@@ -3833,7 +4274,7 @@
         <v>0.2009493670886076</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00161515049914232</v>
+        <v>0.001656122560368622</v>
       </c>
       <c r="G5" t="n">
         <v>0.02333184572108621</v>
@@ -3846,10 +4287,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.05973542016023849</v>
+        <v>0.05909023886759068</v>
       </c>
       <c r="C6" t="n">
-        <v>0.06163465832961143</v>
+        <v>0.06099447513812155</v>
       </c>
       <c r="D6" t="n">
         <v>0.180910792264504</v>
@@ -3858,7 +4299,7 @@
         <v>0.1884057971014493</v>
       </c>
       <c r="F6" t="n">
-        <v>0.001899238169372937</v>
+        <v>0.001904236270530865</v>
       </c>
       <c r="G6" t="n">
         <v>0.007495004836945235</v>
@@ -3867,125 +4308,150 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Lima </t>
+          <t>__MISSING__</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.004881684367430594</v>
+        <v>0.01080064877617222</v>
       </c>
       <c r="C7" t="n">
-        <v>0.004242965609647164</v>
+        <v>0.01038674033149171</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1755725190839695</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1578947368421053</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0006387187577834305</v>
+        <v>-0.000413908444680507</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0176777822418642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Centro </t>
+          <t xml:space="preserve"> Lima </t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.001565120178870878</v>
+        <v>0.004828959009141846</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002009825815096025</v>
+        <v>0.004198895027624309</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1755725190839695</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.1578947368421053</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0004447056362251475</v>
+        <v>-0.0006300639815175367</v>
       </c>
       <c r="G8" t="n">
-        <v>0.05555555555555555</v>
+        <v>-0.0176777822418642</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Norte </t>
+          <t xml:space="preserve"> Centro </t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.002273150735979132</v>
+        <v>0.001548215865526393</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0008932559178204555</v>
+        <v>0.001988950276243094</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2131147540983606</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="E9" t="n">
-        <v>0.25</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.001379894818158676</v>
+        <v>0.0004407344107167008</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03688524590163936</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Sur </t>
+          <t xml:space="preserve"> Norte </t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.00160238494503447</v>
+        <v>0.002248599233264524</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0006699419383653417</v>
+        <v>0.0008839779005524862</v>
       </c>
       <c r="D10" t="n">
-        <v>0.06976744186046512</v>
+        <v>0.2131147540983606</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.0009324430066691282</v>
+        <v>-0.001364621332712037</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.06976744186046512</v>
+        <v>0.03688524590163936</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Oriente </t>
+          <t xml:space="preserve"> Sur </t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0004099124277995156</v>
+        <v>0.001585078148038927</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0004466279589102278</v>
+        <v>0.0006629834254143647</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.06976744186046512</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>3.67155311107122e-05</v>
+        <v>-0.0009220947226245619</v>
       </c>
       <c r="G11" t="n">
+        <v>-0.06976744186046512</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Oriente </t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.000405485107637865</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0004419889502762431</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.650384263837814e-05</v>
+      </c>
+      <c r="G12" t="n">
         <v>-0.4545454545454545</v>
       </c>
     </row>
@@ -4000,7 +4466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4052,10 +4518,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4466239857068414</v>
+        <v>0.4423105278678856</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4397147314464007</v>
+        <v>0.4360220994475138</v>
       </c>
       <c r="D2" t="n">
         <v>0.1805150429202433</v>
@@ -4064,7 +4530,7 @@
         <v>0.1728332488596047</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.006909254260440645</v>
+        <v>-0.006288428420371805</v>
       </c>
       <c r="G2" t="n">
         <v>-0.00768179406063868</v>
@@ -4077,10 +4543,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2955036105114271</v>
+        <v>0.2926496608670009</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3095609538667261</v>
+        <v>0.3069613259668508</v>
       </c>
       <c r="D3" t="n">
         <v>0.1774782718226477</v>
@@ -4089,7 +4555,7 @@
         <v>0.1850251979841613</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01405734335529901</v>
+        <v>0.01431166509984994</v>
       </c>
       <c r="G3" t="n">
         <v>0.007546926161513562</v>
@@ -4102,10 +4568,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2475247524752475</v>
+        <v>0.2451341787083456</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2431468687318921</v>
+        <v>0.2411049723756906</v>
       </c>
       <c r="D4" t="n">
         <v>0.173984962406015</v>
@@ -4114,7 +4580,7 @@
         <v>0.1869844179651696</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.004377883743355376</v>
+        <v>-0.004029206332654994</v>
       </c>
       <c r="G4" t="n">
         <v>0.01299945555915452</v>
@@ -4123,75 +4589,100 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> B </t>
+          <t>__MISSING__</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.005062160351373483</v>
+        <v>0.009657918018283692</v>
       </c>
       <c r="C5" t="n">
-        <v>0.004457321149988857</v>
+        <v>0.008397790055248619</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1764705882352941</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0006048392013846262</v>
+        <v>-0.001260127963035073</v>
       </c>
       <c r="G5" t="n">
-        <v>0.02352941176470588</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A </t>
+          <t xml:space="preserve"> B </t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001935531899054567</v>
+        <v>0.005013270421704512</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001782928459995543</v>
+        <v>0.004419889502762431</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1346153846153846</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="E6" t="n">
-        <v>0.125</v>
+        <v>0.2</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0001526034390590242</v>
+        <v>-0.0005933809189420805</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.009615384615384609</v>
+        <v>0.02352941176470588</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t xml:space="preserve"> A </t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.001916838690651725</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.001767955801104972</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1346153846153846</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.0001488828895467528</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-0.009615384615384609</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t xml:space="preserve"> C </t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.003349959056055981</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.001337196344996657</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="B8" t="n">
+        <v>0.003317605426127986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.001325966850828729</v>
+      </c>
+      <c r="D8" t="n">
         <v>0.1888888888888889</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E8" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="F7" t="n">
-        <v>-0.002012762711059325</v>
-      </c>
-      <c r="G7" t="n">
+      <c r="F8" t="n">
+        <v>-0.001991638575299257</v>
+      </c>
+      <c r="G8" t="n">
         <v>0.1444444444444444</v>
       </c>
     </row>
@@ -4206,7 +4697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4258,10 +4749,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5497448504488397</v>
+        <v>0.5440504276024771</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5458807769591426</v>
+        <v>0.5403314917127072</v>
       </c>
       <c r="D2" t="n">
         <v>0.1760959414594485</v>
@@ -4270,7 +4761,7 @@
         <v>0.1820040899795501</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.003864073489697084</v>
+        <v>-0.003718935889769903</v>
       </c>
       <c r="G2" t="n">
         <v>0.00590814852010163</v>
@@ -4283,10 +4774,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2436771333854807</v>
+        <v>0.241153052196992</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2438044206296048</v>
+        <v>0.2413259668508287</v>
       </c>
       <c r="D3" t="n">
         <v>0.1750229287679609</v>
@@ -4295,7 +4786,7 @@
         <v>0.1730769230769231</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001272872441241413</v>
+        <v>0.0001729146538366755</v>
       </c>
       <c r="G3" t="n">
         <v>-0.001946005691037783</v>
@@ -4308,10 +4799,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1169590643274854</v>
+        <v>0.1157475670893542</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1216789461933467</v>
+        <v>0.1204419889502762</v>
       </c>
       <c r="D4" t="n">
         <v>0.1805732484076433</v>
@@ -4320,7 +4811,7 @@
         <v>0.1577981651376147</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00471988186586135</v>
+        <v>0.004694421860922074</v>
       </c>
       <c r="G4" t="n">
         <v>-0.02277508327002861</v>
@@ -4333,10 +4824,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.07974820277870898</v>
+        <v>0.07892214685933353</v>
       </c>
       <c r="C5" t="n">
-        <v>0.07791917838803304</v>
+        <v>0.07712707182320443</v>
       </c>
       <c r="D5" t="n">
         <v>0.1943017281644092</v>
@@ -4345,7 +4836,7 @@
         <v>0.2206303724928367</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.001829024390675935</v>
+        <v>-0.001795075036129107</v>
       </c>
       <c r="G5" t="n">
         <v>0.02632864432842752</v>
@@ -4354,100 +4845,125 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> TC </t>
+          <t>__MISSING__</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.005885201326032704</v>
+        <v>0.01035830138602182</v>
       </c>
       <c r="C6" t="n">
-        <v>0.007144451886581827</v>
+        <v>0.01016574585635359</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1772151898734177</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.21875</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.001259250560549123</v>
+        <v>-0.0001925555296682317</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04153481012658228</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PL </t>
+          <t xml:space="preserve"> TC </t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.00223488657950609</v>
+        <v>0.005824240636980242</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001786112971645457</v>
+        <v>0.00707182320441989</v>
       </c>
       <c r="D7" t="n">
-        <v>0.15</v>
+        <v>0.1772151898734177</v>
       </c>
       <c r="E7" t="n">
-        <v>0.25</v>
+        <v>0.21875</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.0004487736078606333</v>
+        <v>0.001247582567439648</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1</v>
+        <v>0.04153481012658228</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hipotecario </t>
+          <t xml:space="preserve"> PL </t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.001005698960777741</v>
+        <v>0.002211736950751991</v>
       </c>
       <c r="C8" t="n">
-        <v>0.001339584728734092</v>
+        <v>0.001767955801104972</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.15</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0003338857679563519</v>
+        <v>-0.0004437811496470184</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.05555555555555555</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Hipotecario </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0009952816278383958</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.001325966850828729</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0003306852229903335</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Pyme </t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0.0007449621931686967</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.0004465282429113642</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B10" t="n">
+        <v>0.0007372456502506635</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0004419889502762431</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.05</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="n">
-        <v>-0.0002984339502573325</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="F10" t="n">
+        <v>-0.0002952566999744204</v>
+      </c>
+      <c r="G10" t="n">
         <v>-0.05</v>
       </c>
     </row>

</xml_diff>